<commit_message>
fixed q 7, done
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\emmal\Documents\NSS\Projects\lookups-budget-emmydoore\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A54861-8C44-415F-B6EE-3FA578435E42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E709FEB-DDD8-40D9-940F-AD433D175FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30828" yWindow="-2676" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="91">
   <si>
     <t>Department</t>
   </si>
@@ -304,6 +304,9 @@
   </si>
   <si>
     <t>Actual spending amount - budget amount for fiscal year 2019</t>
+  </si>
+  <si>
+    <t>Question 7</t>
   </si>
 </sst>
 </file>
@@ -1840,16 +1843,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>33337</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>522605</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>146367</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>85</xdr:row>
-      <xdr:rowOff>109537</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>469265</xdr:colOff>
+      <xdr:row>101</xdr:row>
+      <xdr:rowOff>39687</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2176,26 +2179,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F104" sqref="F104"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="J56" sqref="J56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="32.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.85546875" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="15.85546875" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" customWidth="1"/>
-    <col min="14" max="15" width="17.85546875" customWidth="1"/>
-    <col min="16" max="17" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.81640625" customWidth="1"/>
+    <col min="6" max="6" width="30.26953125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.54296875" customWidth="1"/>
+    <col min="8" max="8" width="26.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="15.81640625" customWidth="1"/>
+    <col min="13" max="13" width="15.453125" customWidth="1"/>
+    <col min="14" max="15" width="17.81640625" customWidth="1"/>
+    <col min="16" max="17" width="13.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2245,7 +2248,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -2304,7 +2307,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2422,7 +2425,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -2481,7 +2484,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -2540,7 +2543,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2599,7 +2602,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2658,7 +2661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -2717,7 +2720,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -2776,7 +2779,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>25</v>
       </c>
@@ -2835,7 +2838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>26</v>
       </c>
@@ -2894,7 +2897,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -2953,7 +2956,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -3012,7 +3015,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -3071,7 +3074,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -3130,7 +3133,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>31</v>
       </c>
@@ -3189,7 +3192,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -3248,7 +3251,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>33</v>
       </c>
@@ -3307,7 +3310,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -3366,7 +3369,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -3425,7 +3428,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -3484,7 +3487,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>37</v>
       </c>
@@ -3543,7 +3546,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>38</v>
       </c>
@@ -3602,7 +3605,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>39</v>
       </c>
@@ -3661,7 +3664,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -3720,7 +3723,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -3779,7 +3782,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>42</v>
       </c>
@@ -3838,7 +3841,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>43</v>
       </c>
@@ -3897,7 +3900,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>44</v>
       </c>
@@ -3956,7 +3959,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -4015,7 +4018,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>46</v>
       </c>
@@ -4074,7 +4077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>47</v>
       </c>
@@ -4133,7 +4136,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>48</v>
       </c>
@@ -4192,7 +4195,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -4251,7 +4254,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>50</v>
       </c>
@@ -4310,7 +4313,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>51</v>
       </c>
@@ -4369,7 +4372,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>52</v>
       </c>
@@ -4428,7 +4431,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>53</v>
       </c>
@@ -4487,7 +4490,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>54</v>
       </c>
@@ -4546,7 +4549,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -4605,7 +4608,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>56</v>
       </c>
@@ -4664,7 +4667,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>57</v>
       </c>
@@ -4723,7 +4726,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -4782,7 +4785,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>59</v>
       </c>
@@ -4841,7 +4844,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>60</v>
       </c>
@@ -4900,7 +4903,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>61</v>
       </c>
@@ -4959,7 +4962,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>62</v>
       </c>
@@ -5018,7 +5021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>63</v>
       </c>
@@ -5077,7 +5080,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>64</v>
       </c>
@@ -5136,7 +5139,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>65</v>
       </c>
@@ -5195,7 +5198,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>66</v>
       </c>
@@ -5254,12 +5257,15 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="2" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F54" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>0</v>
       </c>
@@ -5272,115 +5278,218 @@
       <c r="D55" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F55" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>24</v>
       </c>
       <c r="B56">
-        <f t="shared" ref="B56:B57" si="9">VLOOKUP($A56,$A$1:$P$52,MATCH(B$55,$A$1:$P$1))</f>
+        <f>VLOOKUP(A56,$A$1:$P$52,4)</f>
         <v>36209.630000000005</v>
       </c>
       <c r="C56">
-        <f t="shared" ref="C56:D61" si="10">VLOOKUP($A56,$A$1:$P$52,MATCH(C$55,$A$1:$P$1))</f>
+        <f>VLOOKUP($A56,$A$1:$P$52,9)</f>
         <v>27292.159999999974</v>
       </c>
       <c r="D56">
-        <f t="shared" si="10"/>
+        <f>VLOOKUP($A56,$A$1:$P$52,14)</f>
         <v>9181.0800000000163</v>
       </c>
-    </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
+        <v>24</v>
+      </c>
+      <c r="G56">
+        <f t="shared" ref="G56:I61" si="9">VLOOKUP($A56,$A$1:$P$52,MATCH(G$55,$A$1:$P$1))</f>
+        <v>36209.630000000005</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="9"/>
+        <v>27292.159999999974</v>
+      </c>
+      <c r="I56">
+        <f t="shared" si="9"/>
+        <v>9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>25</v>
       </c>
       <c r="B57">
+        <f t="shared" ref="B57:B61" si="10">VLOOKUP(A57,$A$1:$P$52,4)</f>
+        <v>0</v>
+      </c>
+      <c r="C57">
+        <f t="shared" ref="C57:C61" si="11">VLOOKUP($A57,$A$1:$P$52,9)</f>
+        <v>0</v>
+      </c>
+      <c r="D57">
+        <f t="shared" ref="D57:D61" si="12">VLOOKUP($A57,$A$1:$P$52,14)</f>
+        <v>311228.08999999997</v>
+      </c>
+      <c r="F57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G57">
         <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="C57">
-        <f t="shared" si="10"/>
-        <v>0</v>
-      </c>
-      <c r="D57">
-        <f t="shared" si="10"/>
+      <c r="H57">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <f t="shared" si="9"/>
         <v>311228.08999999997</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>32</v>
       </c>
       <c r="B58">
-        <f>VLOOKUP($A58,$A$1:$P$52,MATCH(B$55,$A$1:$P$1))</f>
+        <f t="shared" si="10"/>
         <v>149396.10000000987</v>
       </c>
       <c r="C58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>189254.06000000006</v>
       </c>
       <c r="D58">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>374962.91000000015</v>
       </c>
-    </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
+        <v>32</v>
+      </c>
+      <c r="G58">
+        <f>VLOOKUP($A58,$A$1:$P$52,MATCH(G$55,$A$1:$P$1))</f>
+        <v>149396.10000000987</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="9"/>
+        <v>189254.06000000006</v>
+      </c>
+      <c r="I58">
+        <f t="shared" si="9"/>
+        <v>374962.91000000015</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>38</v>
       </c>
       <c r="B59">
-        <f t="shared" ref="B59:B61" si="11">VLOOKUP($A59,$A$1:$P$52,MATCH(B$55,$A$1:$P$1))</f>
+        <f t="shared" si="10"/>
         <v>12230.810000000056</v>
       </c>
       <c r="C59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>45485.580000000075</v>
       </c>
       <c r="D59">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>72.879999999888241</v>
       </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
+        <v>38</v>
+      </c>
+      <c r="G59">
+        <f t="shared" ref="G59:G61" si="13">VLOOKUP($A59,$A$1:$P$52,MATCH(G$55,$A$1:$P$1))</f>
+        <v>12230.810000000056</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="9"/>
+        <v>45485.580000000075</v>
+      </c>
+      <c r="I59">
+        <f t="shared" si="9"/>
+        <v>72.879999999888241</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>39</v>
       </c>
       <c r="B60">
+        <f t="shared" si="10"/>
+        <v>4950.4699999999721</v>
+      </c>
+      <c r="C60">
         <f t="shared" si="11"/>
+        <v>8005.7900000010268</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="12"/>
+        <v>1724.9000000000233</v>
+      </c>
+      <c r="F60" t="s">
+        <v>39</v>
+      </c>
+      <c r="G60">
+        <f t="shared" si="13"/>
         <v>4950.4699999999721</v>
       </c>
-      <c r="C60">
-        <f t="shared" si="10"/>
+      <c r="H60">
+        <f t="shared" si="9"/>
         <v>8005.7900000010268</v>
       </c>
-      <c r="D60">
-        <f t="shared" si="10"/>
+      <c r="I60">
+        <f t="shared" si="9"/>
         <v>1724.9000000000233</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>55</v>
       </c>
       <c r="B61">
+        <f t="shared" si="10"/>
+        <v>184239.79000001028</v>
+      </c>
+      <c r="C61">
         <f t="shared" si="11"/>
+        <v>133456.33000001032</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="12"/>
+        <v>82077.349999999627</v>
+      </c>
+      <c r="F61" t="s">
+        <v>55</v>
+      </c>
+      <c r="G61">
+        <f t="shared" si="13"/>
         <v>184239.79000001028</v>
       </c>
-      <c r="C61">
-        <f t="shared" si="10"/>
+      <c r="H61">
+        <f t="shared" si="9"/>
         <v>133456.33000001032</v>
       </c>
-      <c r="D61">
-        <f t="shared" si="10"/>
+      <c r="I61">
+        <f t="shared" si="9"/>
         <v>82077.349999999627</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="7" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="F63" s="7"/>
+    </row>
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>0</v>
       </c>
@@ -5393,115 +5502,218 @@
       <c r="D64" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F64" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G64" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>24</v>
       </c>
       <c r="B65">
-        <f>VLOOKUP($A65,$A$1:$P$52,MATCH(B$64,$A$1:$P$1))</f>
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$D$2:$D$52)</f>
         <v>36209.630000000005</v>
       </c>
       <c r="C65">
-        <f t="shared" ref="C65:D70" si="12">VLOOKUP($A65,$A$1:$P$52,MATCH(C$64,$A$1:$P$1))</f>
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$I$2:$I$52)</f>
         <v>27292.159999999974</v>
       </c>
       <c r="D65">
-        <f t="shared" si="12"/>
+        <f>_xlfn.XLOOKUP(A65,$A$2:$A$52,$N$2:$N$52)</f>
         <v>9181.0800000000163</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
+        <v>24</v>
+      </c>
+      <c r="G65">
+        <f>VLOOKUP($A65,$A$1:$P$52,MATCH(G$64,$A$1:$P$1))</f>
+        <v>36209.630000000005</v>
+      </c>
+      <c r="H65">
+        <f t="shared" ref="H65:I70" si="14">VLOOKUP($A65,$A$1:$P$52,MATCH(H$64,$A$1:$P$1))</f>
+        <v>27292.159999999974</v>
+      </c>
+      <c r="I65">
+        <f t="shared" si="14"/>
+        <v>9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>25</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B70" si="13">VLOOKUP($A66,$A$1:$P$52,MATCH(B$64,$A$1:$P$1))</f>
+        <f t="shared" ref="B66:B70" si="15">_xlfn.XLOOKUP(A66,$A$2:$A$52,$D$2:$D$52)</f>
         <v>0</v>
       </c>
       <c r="C66">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="C66:C70" si="16">_xlfn.XLOOKUP(A66,$A$2:$A$52,$I$2:$I$52)</f>
         <v>0</v>
       </c>
       <c r="D66">
-        <f t="shared" si="12"/>
+        <f t="shared" ref="D66:D70" si="17">_xlfn.XLOOKUP(A66,$A$2:$A$52,$N$2:$N$52)</f>
         <v>311228.08999999997</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
+        <v>25</v>
+      </c>
+      <c r="G66">
+        <f t="shared" ref="G66:G70" si="18">VLOOKUP($A66,$A$1:$P$52,MATCH(G$64,$A$1:$P$1))</f>
+        <v>0</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="I66">
+        <f t="shared" si="14"/>
+        <v>311228.08999999997</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>32</v>
       </c>
       <c r="B67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>149396.10000000987</v>
       </c>
       <c r="C67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>189254.06000000006</v>
       </c>
       <c r="D67">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>374962.91000000015</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>32</v>
+      </c>
+      <c r="G67">
+        <f t="shared" si="18"/>
+        <v>149396.10000000987</v>
+      </c>
+      <c r="H67">
+        <f t="shared" si="14"/>
+        <v>189254.06000000006</v>
+      </c>
+      <c r="I67">
+        <f t="shared" si="14"/>
+        <v>374962.91000000015</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>38</v>
       </c>
       <c r="B68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>12230.810000000056</v>
       </c>
       <c r="C68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>45485.580000000075</v>
       </c>
       <c r="D68">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>72.879999999888241</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
+        <v>38</v>
+      </c>
+      <c r="G68">
+        <f t="shared" si="18"/>
+        <v>12230.810000000056</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="14"/>
+        <v>45485.580000000075</v>
+      </c>
+      <c r="I68">
+        <f t="shared" si="14"/>
+        <v>72.879999999888241</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>39</v>
       </c>
       <c r="B69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4950.4699999999721</v>
       </c>
       <c r="C69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>8005.7900000010268</v>
       </c>
       <c r="D69">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>1724.9000000000233</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
+        <v>39</v>
+      </c>
+      <c r="G69">
+        <f t="shared" si="18"/>
+        <v>4950.4699999999721</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="14"/>
+        <v>8005.7900000010268</v>
+      </c>
+      <c r="I69">
+        <f t="shared" si="14"/>
+        <v>1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>55</v>
       </c>
       <c r="B70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>184239.79000001028</v>
       </c>
       <c r="C70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="16"/>
         <v>133456.33000001032</v>
       </c>
       <c r="D70">
-        <f t="shared" si="12"/>
+        <f t="shared" si="17"/>
         <v>82077.349999999627</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
+        <v>55</v>
+      </c>
+      <c r="G70">
+        <f t="shared" si="18"/>
+        <v>184239.79000001028</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="14"/>
+        <v>133456.33000001032</v>
+      </c>
+      <c r="I70">
+        <f t="shared" si="14"/>
+        <v>82077.349999999627</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="7" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F72" s="7"/>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>0</v>
       </c>
@@ -5514,121 +5726,217 @@
       <c r="D73" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F73" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>24</v>
       </c>
       <c r="B74">
-        <f>VLOOKUP($A74,$A$1:$P$52,MATCH(B$73,$A$1:$P$1))</f>
+        <f t="shared" ref="B74:B78" si="19">INDEX($D$2:$D$52,MATCH($A74,$A$2:$A$52,0))</f>
         <v>36209.630000000005</v>
       </c>
       <c r="C74">
-        <f t="shared" ref="C74:D79" si="14">VLOOKUP($A74,$A$1:$P$52,MATCH(C$73,$A$1:$P$1))</f>
+        <f t="shared" ref="C74:C78" si="20">INDEX($I$2:$I$52,MATCH($A74,$A$2:$A$52,0))</f>
         <v>27292.159999999974</v>
       </c>
       <c r="D74">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="D74:D78" si="21">INDEX($N$2:$N$52,MATCH($A74,$A$2:$A$52,0))</f>
         <v>9181.0800000000163</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
+        <v>24</v>
+      </c>
+      <c r="G74">
+        <f>VLOOKUP($A74,$A$1:$P$52,MATCH(G$73,$A$1:$P$1))</f>
+        <v>36209.630000000005</v>
+      </c>
+      <c r="H74">
+        <f t="shared" ref="H74:I79" si="22">VLOOKUP($A74,$A$1:$P$52,MATCH(H$73,$A$1:$P$1))</f>
+        <v>27292.159999999974</v>
+      </c>
+      <c r="I74">
+        <f t="shared" si="22"/>
+        <v>9181.0800000000163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>25</v>
       </c>
       <c r="B75">
-        <f t="shared" ref="B75:B79" si="15">VLOOKUP($A75,$A$1:$P$52,MATCH(B$73,$A$1:$P$1))</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="C75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="D75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>311228.08999999997</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
+        <v>25</v>
+      </c>
+      <c r="G75">
+        <f t="shared" ref="G75:G79" si="23">VLOOKUP($A75,$A$1:$P$52,MATCH(G$73,$A$1:$P$1))</f>
+        <v>0</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="22"/>
+        <v>0</v>
+      </c>
+      <c r="I75">
+        <f t="shared" si="22"/>
+        <v>311228.08999999997</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>32</v>
       </c>
       <c r="B76">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>149396.10000000987</v>
       </c>
       <c r="C76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>189254.06000000006</v>
       </c>
       <c r="D76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>374962.91000000015</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
+        <v>32</v>
+      </c>
+      <c r="G76">
+        <f t="shared" si="23"/>
+        <v>149396.10000000987</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="22"/>
+        <v>189254.06000000006</v>
+      </c>
+      <c r="I76">
+        <f t="shared" si="22"/>
+        <v>374962.91000000015</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>38</v>
       </c>
       <c r="B77">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>12230.810000000056</v>
       </c>
       <c r="C77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>45485.580000000075</v>
       </c>
       <c r="D77">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>72.879999999888241</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
+        <v>38</v>
+      </c>
+      <c r="G77">
+        <f t="shared" si="23"/>
+        <v>12230.810000000056</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="22"/>
+        <v>45485.580000000075</v>
+      </c>
+      <c r="I77">
+        <f t="shared" si="22"/>
+        <v>72.879999999888241</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>39</v>
       </c>
       <c r="B78">
-        <f t="shared" si="15"/>
+        <f t="shared" si="19"/>
         <v>4950.4699999999721</v>
       </c>
       <c r="C78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="20"/>
         <v>8005.7900000010268</v>
       </c>
       <c r="D78">
-        <f t="shared" si="14"/>
+        <f t="shared" si="21"/>
         <v>1724.9000000000233</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
+        <v>39</v>
+      </c>
+      <c r="G78">
+        <f t="shared" si="23"/>
+        <v>4950.4699999999721</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="22"/>
+        <v>8005.7900000010268</v>
+      </c>
+      <c r="I78">
+        <f t="shared" si="22"/>
+        <v>1724.9000000000233</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>55</v>
       </c>
       <c r="B79">
-        <f t="shared" si="15"/>
+        <f>INDEX($D$2:$D$52,MATCH($A79,$A$2:$A$52,0))</f>
         <v>184239.79000001028</v>
       </c>
       <c r="C79">
-        <f t="shared" si="14"/>
+        <f>INDEX($I$2:$I$52,MATCH($A79,$A$2:$A$52,0))</f>
         <v>133456.33000001032</v>
       </c>
       <c r="D79">
-        <f t="shared" si="14"/>
+        <f>INDEX($N$2:$N$52,MATCH($A79,$A$2:$A$52,0))</f>
         <v>82077.349999999627</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80">
-        <f>INDEX($D$2:$D$52,MATCH(A79,$A$2:$A$52,0))</f>
+      <c r="F79" t="s">
+        <v>55</v>
+      </c>
+      <c r="G79">
+        <f t="shared" si="23"/>
         <v>184239.79000001028</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H79">
+        <f t="shared" si="22"/>
+        <v>133456.33000001032</v>
+      </c>
+      <c r="I79">
+        <f t="shared" si="22"/>
+        <v>82077.349999999627</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A81" s="7" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -5636,7 +5944,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B83" s="1" t="s">
         <v>71</v>
       </c>
@@ -5644,7 +5952,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>73</v>
       </c>
@@ -5657,7 +5965,7 @@
         <v>5772288.3300000001</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>74</v>
       </c>
@@ -5670,7 +5978,7 @@
         <v>314622.06000000983</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>75</v>
       </c>
@@ -5683,12 +5991,12 @@
         <v>150323.33000000007</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A88" s="7" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>77</v>
       </c>
@@ -5704,7 +6012,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B90" s="8" t="s">
         <v>0</v>
       </c>
@@ -5724,12 +6032,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>73</v>
       </c>
       <c r="B91" t="str">
-        <f>_xlfn.XLOOKUP(B89,$F$2:$F$52,$A$2:$A$52)</f>
+        <f>_xlfn.XLOOKUP(B$89,$F$2:$F$52,$A$2:$A$52)</f>
         <v>Clerk and Master - Chancery</v>
       </c>
       <c r="C91" s="5">
@@ -5753,12 +6061,12 @@
         <v>9.5782760864849215E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>74</v>
       </c>
       <c r="B92" t="str">
-        <f>_xlfn.XLOOKUP(B89,$K$2:$K$52,$A$2:$A$52)</f>
+        <f>_xlfn.XLOOKUP(B$89,$K$2:$K$52,$A$2:$A$52)</f>
         <v>Metropolitan Clerk</v>
       </c>
       <c r="C92" s="5">
@@ -5782,12 +6090,12 @@
         <v>0.13918241656366656</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>75</v>
       </c>
       <c r="B93" t="str">
-        <f>_xlfn.XLOOKUP(B89,$P$2:$P$52,$A$2:$A$52)</f>
+        <f>_xlfn.XLOOKUP(B$89,$P$2:$P$52,$A$2:$A$52)</f>
         <v>Community Oversight Board</v>
       </c>
       <c r="C93" s="5">
@@ -5811,12 +6119,12 @@
         <v>0.12882667147667154</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A95" s="7" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>77</v>
       </c>
@@ -5832,7 +6140,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B97" s="8" t="s">
         <v>0</v>
       </c>
@@ -5852,7 +6160,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>73</v>
       </c>
@@ -5869,7 +6177,7 @@
         <v>Circuit Court Clerk</v>
       </c>
       <c r="E98" s="5">
-        <f t="shared" ref="E98:G98" si="16">INDEX($E$2:$E$52,MATCH(D96,$F$2:$F$52,0))</f>
+        <f t="shared" ref="E98:G98" si="24">INDEX($E$2:$E$52,MATCH(D96,$F$2:$F$52,0))</f>
         <v>0.11502817362571344</v>
       </c>
       <c r="F98" t="str">
@@ -5877,12 +6185,12 @@
         <v>Internal Audit</v>
       </c>
       <c r="G98" s="5">
-        <f t="shared" si="16"/>
+        <f t="shared" si="24"/>
         <v>9.5782760864849215E-2</v>
       </c>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>74</v>
       </c>
@@ -5899,7 +6207,7 @@
         <v>Internal Audit</v>
       </c>
       <c r="E99" s="5">
-        <f t="shared" ref="E99:G99" si="17">INDEX($J$2:$J$52,MATCH(D96,$K$2:$K$52,0))</f>
+        <f t="shared" ref="E99:G99" si="25">INDEX($J$2:$J$52,MATCH(D96,$K$2:$K$52,0))</f>
         <v>0.17103239309050916</v>
       </c>
       <c r="F99" t="str">
@@ -5907,12 +6215,12 @@
         <v>Office of Family Safety</v>
       </c>
       <c r="G99" s="5">
-        <f t="shared" si="17"/>
+        <f t="shared" si="25"/>
         <v>0.13918241656366656</v>
       </c>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>75</v>
       </c>
@@ -5929,7 +6237,7 @@
         <v>Clerk and Master - Chancery</v>
       </c>
       <c r="E100" s="5">
-        <f t="shared" ref="E100:G100" si="18">INDEX($O$2:$O$52,MATCH(D$96,$P$2:$P$52,0))</f>
+        <f t="shared" ref="E100:G100" si="26">INDEX($O$2:$O$52,MATCH(D$96,$P$2:$P$52,0))</f>
         <v>0.15295680364719175</v>
       </c>
       <c r="F100" t="str">
@@ -5937,13 +6245,13 @@
         <v>Election Commission</v>
       </c>
       <c r="G100" s="5">
-        <f t="shared" si="18"/>
+        <f t="shared" si="26"/>
         <v>0.12882667147667154</v>
       </c>
       <c r="I100" s="4"/>
     </row>
   </sheetData>
-  <dataValidations count="3">
+  <dataValidations disablePrompts="1" count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A83" xr:uid="{0ECE0BAD-DC74-4E7B-8842-0609702F3664}">
       <formula1>$A$2:$A$52</formula1>
     </dataValidation>
@@ -5968,13 +6276,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="52.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5982,7 +6290,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -5990,7 +6298,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -5998,7 +6306,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -6006,7 +6314,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -6014,7 +6322,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
@@ -6022,7 +6330,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -6030,7 +6338,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>11</v>
       </c>
@@ -6038,7 +6346,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>12</v>
       </c>
@@ -6046,7 +6354,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" s="2" t="s">
         <v>13</v>
       </c>

</xml_diff>